<commit_message>
Added image extractor from an excel chart. Added 5 examples
</commit_message>
<xml_diff>
--- a/GenerateApp/tables/Data/1/source.xlsx
+++ b/GenerateApp/tables/Data/1/source.xlsx
@@ -68,7 +68,7 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:t>Bar Chart</a:t>
+              <a:t/>
             </a:r>
           </a:p>
         </rich>
@@ -88,12 +88,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Sheet1'!$A$1:$A$6</f>
+              <f>'Sheet1'!$A$1:$A$7</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Sheet1'!$B$1:$B$6</f>
+              <f>'Sheet1'!$B$1:$B$7</f>
             </numRef>
           </val>
         </ser>
@@ -479,7 +479,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -492,7 +492,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="n">
-        <v>543</v>
+        <v>893</v>
       </c>
     </row>
     <row r="2">
@@ -500,7 +500,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="n">
-        <v>220</v>
+        <v>306</v>
       </c>
     </row>
     <row r="3">
@@ -508,7 +508,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="n">
-        <v>495</v>
+        <v>510</v>
       </c>
     </row>
     <row r="4">
@@ -516,7 +516,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>245</v>
+        <v>572</v>
       </c>
     </row>
     <row r="5">
@@ -524,7 +524,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="n">
-        <v>490</v>
+        <v>902</v>
       </c>
     </row>
     <row r="6">
@@ -532,7 +532,15 @@
         <v>6</v>
       </c>
       <c r="B6" t="n">
-        <v>346</v>
+        <v>826</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>7</v>
+      </c>
+      <c r="B7" t="n">
+        <v>710</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Moved table creation and image export to functions. Fixed CWD change.
</commit_message>
<xml_diff>
--- a/GenerateApp/tables/Data/1/source.xlsx
+++ b/GenerateApp/tables/Data/1/source.xlsx
@@ -492,7 +492,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="n">
-        <v>893</v>
+        <v>537</v>
       </c>
     </row>
     <row r="2">
@@ -500,7 +500,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="n">
-        <v>306</v>
+        <v>377</v>
       </c>
     </row>
     <row r="3">
@@ -508,7 +508,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="n">
-        <v>510</v>
+        <v>687</v>
       </c>
     </row>
     <row r="4">
@@ -516,7 +516,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>572</v>
+        <v>468</v>
       </c>
     </row>
     <row r="5">
@@ -524,7 +524,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="n">
-        <v>902</v>
+        <v>641</v>
       </c>
     </row>
     <row r="6">
@@ -532,7 +532,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="n">
-        <v>826</v>
+        <v>436</v>
       </c>
     </row>
     <row r="7">
@@ -540,7 +540,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="n">
-        <v>710</v>
+        <v>572</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added randomization to the generation algorithm. Added generated examples Added gitignore
</commit_message>
<xml_diff>
--- a/GenerateApp/tables/Data/1/source.xlsx
+++ b/GenerateApp/tables/Data/1/source.xlsx
@@ -57,7 +57,7 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <style val="4"/>
+  <style val="8"/>
   <chart>
     <title>
       <tx>
@@ -75,6 +75,14 @@
       </tx>
     </title>
     <plotArea>
+      <layout>
+        <manualLayout>
+          <wMode val="factor"/>
+          <hMode val="factor"/>
+          <w val="0.85"/>
+          <h val="0.85"/>
+        </manualLayout>
+      </layout>
       <barChart>
         <barDir val="col"/>
         <grouping val="clustered"/>
@@ -88,12 +96,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Sheet1'!$A$1:$A$7</f>
+              <f>'Sheet1'!$A$1:$A$12</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Sheet1'!$B$1:$B$7</f>
+              <f>'Sheet1'!$B$1:$B$12</f>
             </numRef>
           </val>
         </ser>
@@ -479,7 +487,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -488,59 +496,123 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="n">
-        <v>1</v>
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>December 2015</t>
+        </is>
       </c>
       <c r="B1" t="n">
-        <v>537</v>
+        <v>578</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>2</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>January 2016</t>
+        </is>
       </c>
       <c r="B2" t="n">
-        <v>377</v>
+        <v>527</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>3</v>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>February 2016</t>
+        </is>
       </c>
       <c r="B3" t="n">
-        <v>687</v>
+        <v>424</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>4</v>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>March 2016</t>
+        </is>
       </c>
       <c r="B4" t="n">
-        <v>468</v>
+        <v>427</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
-        <v>5</v>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>April 2016</t>
+        </is>
       </c>
       <c r="B5" t="n">
-        <v>641</v>
+        <v>538</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
-        <v>6</v>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>May 2016</t>
+        </is>
       </c>
       <c r="B6" t="n">
-        <v>436</v>
+        <v>557</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
-        <v>7</v>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>June 2016</t>
+        </is>
       </c>
       <c r="B7" t="n">
-        <v>572</v>
+        <v>488</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>July 2016</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>August 2016</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>September 2016</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>October 2016</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>November 2016</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>448</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new console parameter for maximum number of columns. Added more examples
</commit_message>
<xml_diff>
--- a/GenerateApp/tables/Data/1/source.xlsx
+++ b/GenerateApp/tables/Data/1/source.xlsx
@@ -57,7 +57,7 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <style val="8"/>
+  <style val="2"/>
   <chart>
     <title>
       <tx>
@@ -96,12 +96,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Sheet1'!$A$1:$A$12</f>
+              <f>'Sheet1'!$A$1:$A$13</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Sheet1'!$B$1:$B$12</f>
+              <f>'Sheet1'!$B$1:$B$13</f>
             </numRef>
           </val>
         </ser>
@@ -487,7 +487,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -498,121 +498,131 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>December 2015</t>
+          <t>October 2018</t>
         </is>
       </c>
       <c r="B1" t="n">
-        <v>578</v>
+        <v>497</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>January 2016</t>
+          <t>November 2018</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>527</v>
+        <v>373</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>February 2016</t>
+          <t>December 2018</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>424</v>
+        <v>568</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>March 2016</t>
+          <t>January 2019</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>427</v>
+        <v>554</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>April 2016</t>
+          <t>February 2019</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>538</v>
+        <v>581</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>May 2016</t>
+          <t>March 2019</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>557</v>
+        <v>670</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>June 2016</t>
+          <t>April 2019</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>488</v>
+        <v>612</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>July 2016</t>
+          <t>May 2019</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>454</v>
+        <v>629</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>August 2016</t>
+          <t>June 2019</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>651</v>
+        <v>371</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>September 2016</t>
+          <t>July 2019</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>488</v>
+        <v>691</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>October 2016</t>
+          <t>August 2019</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>426</v>
+        <v>404</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>November 2016</t>
+          <t>September 2019</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>448</v>
+        <v>563</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>October 2019</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>519</v>
       </c>
     </row>
   </sheetData>

</xml_diff>